<commit_message>
alternate versions with quartiles and terciles
</commit_message>
<xml_diff>
--- a/MobilityTable_v02.xlsx
+++ b/MobilityTable_v02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fpfeffer/Documents/10 Projects/18 WealthCorrRaceVisual/Analysis/DataPreparation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loy/Documents/Github/wealth-mobility-vis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E825560D-3B55-4845-9C41-9B93E041F03A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58923E7-EAC9-FC4B-A3C2-8AE1B3E3F5D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{4218A992-A353-2C4B-A5CA-736F53E1FD53}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{4218A992-A353-2C4B-A5CA-736F53E1FD53}"/>
   </bookViews>
   <sheets>
     <sheet name="Terciles" sheetId="2" r:id="rId1"/>
@@ -457,7 +457,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:F18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBAB444-E314-4A4F-B9F9-ECF535992F1C}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:G19"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -974,7 +974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D3307F-73A9-014C-9414-1E534D1BAF50}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>